<commit_message>
Revisi Tingkat Pendidikan & APS
</commit_message>
<xml_diff>
--- a/Rekap/RekapAngkaPartisipasiSekolah.xlsx
+++ b/Rekap/RekapAngkaPartisipasiSekolah.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>No</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>16-18 Thn (%)</t>
-  </si>
-  <si>
-    <t>19-24 Thn (%)</t>
   </si>
   <si>
     <t>Pesanggaran</t>
@@ -121,9 +118,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -154,8 +151,86 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -169,39 +244,37 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -209,90 +282,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -307,6 +304,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -319,19 +370,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -343,151 +472,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -544,11 +541,55 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -582,195 +623,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1119,20 +1116,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="5.42857142857143" style="1" customWidth="1"/>
     <col min="2" max="2" width="26.2857142857143" customWidth="1"/>
-    <col min="3" max="6" width="14.7142857142857" customWidth="1"/>
+    <col min="3" max="5" width="14.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="35.25" customHeight="1" spans="1:6">
+    <row r="1" ht="35.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1148,528 +1145,447 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" ht="15.75" spans="1:6">
+    </row>
+    <row r="2" ht="15.75" spans="1:5">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="5">
-        <v>100</v>
+        <v>97.9311281327</v>
       </c>
       <c r="D2" s="5">
-        <v>94.44</v>
+        <v>96.1225360783451</v>
       </c>
       <c r="E2" s="5">
-        <v>88.89</v>
-      </c>
-      <c r="F2" s="5">
-        <v>21.88</v>
-      </c>
-    </row>
-    <row r="3" ht="15.75" spans="1:6">
+        <v>78.8103015454587</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" spans="1:5">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="5">
-        <v>91.18</v>
+        <v>98.5985532707442</v>
       </c>
       <c r="D3" s="5">
-        <v>90.91</v>
+        <v>98.0933313528296</v>
       </c>
       <c r="E3" s="5">
-        <v>86.36</v>
-      </c>
-      <c r="F3" s="5">
-        <v>8.33</v>
-      </c>
-    </row>
-    <row r="4" ht="15.75" spans="1:6">
+        <v>80.2610895175262</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" spans="1:5">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5">
-        <v>100</v>
+        <v>99.4724849479068</v>
       </c>
       <c r="D4" s="5">
-        <v>100</v>
+        <v>97.8048731336726</v>
       </c>
       <c r="E4" s="5">
-        <v>91.67</v>
-      </c>
-      <c r="F4" s="5">
-        <v>35.29</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" spans="1:6">
+        <v>80.5574530833899</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" spans="1:5">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="5">
-        <v>82.35</v>
+        <v>99.0262182942546</v>
       </c>
       <c r="D5" s="5">
-        <v>80</v>
+        <v>98.6634855767358</v>
       </c>
       <c r="E5" s="5">
-        <v>73.33</v>
-      </c>
-      <c r="F5" s="5">
-        <v>21.74</v>
-      </c>
-    </row>
-    <row r="6" ht="15.75" spans="1:6">
+        <v>81.18259845107</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" spans="1:5">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="5">
-        <v>94.59</v>
+        <v>97.2824979741973</v>
       </c>
       <c r="D6" s="5">
-        <v>83.33</v>
+        <v>95.4894358183993</v>
       </c>
       <c r="E6" s="5">
-        <v>83.33</v>
-      </c>
-      <c r="F6" s="5">
-        <v>53.75</v>
-      </c>
-    </row>
-    <row r="7" ht="15.75" spans="1:6">
+        <v>77.7837917287354</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" spans="1:5">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="5">
-        <v>92.31</v>
+        <v>99.4875342001982</v>
       </c>
       <c r="D7" s="5">
-        <v>83.33</v>
+        <v>99.0876471864978</v>
       </c>
       <c r="E7" s="5">
-        <v>75</v>
-      </c>
-      <c r="F7" s="5">
-        <v>24.24</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" spans="1:6">
+        <v>81.5957291290347</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" spans="1:5">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="5">
-        <v>92.31</v>
+        <v>100</v>
       </c>
       <c r="D8" s="5">
-        <v>92.11</v>
+        <v>98.6163650570842</v>
       </c>
       <c r="E8" s="5">
-        <v>84.21</v>
-      </c>
-      <c r="F8" s="5">
-        <v>18.92</v>
-      </c>
-    </row>
-    <row r="9" ht="15.75" spans="1:6">
+        <v>82.4688561945537</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" spans="1:5">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="5">
-        <v>95.24</v>
+        <v>98.034825157895</v>
       </c>
       <c r="D9" s="5">
-        <v>94</v>
+        <v>98.0306706211415</v>
       </c>
       <c r="E9" s="5">
-        <v>87.1</v>
-      </c>
-      <c r="F9" s="5">
-        <v>25.53</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" spans="1:6">
+        <v>80.5081227077229</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" spans="1:5">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="5">
         <v>100</v>
       </c>
       <c r="D10" s="5">
-        <v>100</v>
+        <v>99.6662949068342</v>
       </c>
       <c r="E10" s="5">
-        <v>89.66</v>
-      </c>
-      <c r="F10" s="5">
-        <v>41.86</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75" spans="1:6">
+        <v>85.3439599674588</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" spans="1:5">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="5">
-        <v>100</v>
+        <v>99.1286384863987</v>
       </c>
       <c r="D11" s="5">
-        <v>96.77</v>
+        <v>98.3351436191198</v>
       </c>
       <c r="E11" s="5">
-        <v>88.89</v>
-      </c>
-      <c r="F11" s="5">
-        <v>25.81</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" spans="1:6">
+        <v>80.740338569807</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" spans="1:5">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="5">
-        <v>100</v>
+        <v>98.0130440145755</v>
       </c>
       <c r="D12" s="5">
-        <v>100</v>
+        <v>96.3777543400429</v>
       </c>
       <c r="E12" s="5">
-        <v>87.5</v>
-      </c>
-      <c r="F12" s="5">
-        <v>21.43</v>
-      </c>
-    </row>
-    <row r="13" ht="15.75" spans="1:6">
+        <v>78.4132834488786</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" spans="1:5">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="5">
-        <v>100</v>
+        <v>97.5790512295518</v>
       </c>
       <c r="D13" s="5">
-        <v>88</v>
+        <v>97.0678474400674</v>
       </c>
       <c r="E13" s="5">
-        <v>63.64</v>
-      </c>
-      <c r="F13" s="5">
-        <v>38.71</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" spans="1:6">
+        <v>79.7123418971528</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" spans="1:5">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="5">
-        <v>100</v>
+        <v>98.7199071459218</v>
       </c>
       <c r="D14" s="5">
-        <v>92.86</v>
+        <v>96.9774592685548</v>
       </c>
       <c r="E14" s="5">
-        <v>75</v>
-      </c>
-      <c r="F14" s="5">
-        <v>13.33</v>
-      </c>
-    </row>
-    <row r="15" ht="15.75" spans="1:6">
+        <v>79.1306692602259</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" spans="1:5">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="5">
-        <v>90.48</v>
+        <v>98.8771481740422</v>
       </c>
       <c r="D15" s="5">
-        <v>87.5</v>
+        <v>98.3500312594027</v>
       </c>
       <c r="E15" s="5">
-        <v>84.62</v>
-      </c>
-      <c r="F15" s="5">
-        <v>6.67</v>
-      </c>
-    </row>
-    <row r="16" ht="15.75" spans="1:6">
+        <v>80.8638429560995</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" spans="1:5">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="5">
-        <v>100</v>
+        <v>99.0055479785361</v>
       </c>
       <c r="D16" s="5">
-        <v>100</v>
+        <v>97.5355819809977</v>
       </c>
       <c r="E16" s="5">
-        <v>87.5</v>
-      </c>
-      <c r="F16" s="5">
-        <v>21.43</v>
-      </c>
-    </row>
-    <row r="17" ht="15.75" spans="1:6">
+        <v>80.4060359950349</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" spans="1:5">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="5">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="D17" s="5">
-        <v>76.09</v>
+        <v>98.595470419775</v>
       </c>
       <c r="E17" s="5">
-        <v>63.64</v>
-      </c>
-      <c r="F17" s="5">
-        <v>16.36</v>
-      </c>
-    </row>
-    <row r="18" ht="15.75" spans="1:6">
+        <v>86.1681540371001</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75" spans="1:5">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="5">
-        <v>93.33</v>
+        <v>100</v>
       </c>
       <c r="D18" s="5">
-        <v>87.5</v>
+        <v>98.0116982899647</v>
       </c>
       <c r="E18" s="5">
-        <v>25</v>
-      </c>
-      <c r="F18" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" ht="15.75" spans="1:6">
+        <v>85.6337153350587</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" spans="1:5">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="5">
-        <v>100</v>
+        <v>97.6881865922571</v>
       </c>
       <c r="D19" s="5">
-        <v>100</v>
+        <v>96.8796850839585</v>
       </c>
       <c r="E19" s="5">
-        <v>91.3</v>
-      </c>
-      <c r="F19" s="5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" ht="15.75" spans="1:6">
+        <v>79.7530796183234</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" spans="1:5">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="5">
-        <v>100</v>
+        <v>99.3545189814721</v>
       </c>
       <c r="D20" s="5">
-        <v>83.33</v>
+        <v>99.2053157312475</v>
       </c>
       <c r="E20" s="5">
-        <v>80.95</v>
-      </c>
-      <c r="F20" s="5">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" spans="1:6">
+        <v>81.830035728826</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" spans="1:5">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="5">
-        <v>100</v>
+        <v>97.6456399993159</v>
       </c>
       <c r="D21" s="5">
-        <v>95.24</v>
+        <v>96.1387421257396</v>
       </c>
       <c r="E21" s="5">
-        <v>83.33</v>
-      </c>
-      <c r="F21" s="5">
-        <v>20.69</v>
-      </c>
-    </row>
-    <row r="22" ht="15.75" spans="1:6">
+        <v>78.2315439383658</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" spans="1:5">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="5">
-        <v>88.24</v>
+        <v>98.9277548715103</v>
       </c>
       <c r="D22" s="5">
-        <v>77.78</v>
+        <v>98.8667194598649</v>
       </c>
       <c r="E22" s="5">
-        <v>77.14</v>
-      </c>
-      <c r="F22" s="5">
-        <v>10.53</v>
-      </c>
-    </row>
-    <row r="23" ht="15.75" spans="1:6">
+        <v>81.4853521030271</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" spans="1:5">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" s="5">
-        <v>100</v>
+        <v>99.3543093509044</v>
       </c>
       <c r="D23" s="5">
-        <v>95.83</v>
+        <v>98.6863589187405</v>
       </c>
       <c r="E23" s="5">
-        <v>78.57</v>
-      </c>
-      <c r="F23" s="5">
-        <v>9.09</v>
-      </c>
-    </row>
-    <row r="24" ht="15.75" spans="1:6">
+        <v>81.2540222512306</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" spans="1:5">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="5">
-        <v>100</v>
+        <v>97.5437693426962</v>
       </c>
       <c r="D24" s="5">
-        <v>100</v>
+        <v>96.5115528292741</v>
       </c>
       <c r="E24" s="5">
-        <v>72.73</v>
-      </c>
-      <c r="F24" s="5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" ht="15.75" spans="1:6">
+        <v>78.6876433255483</v>
+      </c>
+    </row>
+    <row r="25" ht="15.75" spans="1:5">
       <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" s="5">
-        <v>100</v>
+        <v>97.179769149413</v>
       </c>
       <c r="D25" s="5">
-        <v>100</v>
+        <v>95.5408981689556</v>
       </c>
       <c r="E25" s="5">
-        <v>87.5</v>
-      </c>
-      <c r="F25" s="5">
-        <v>31.25</v>
-      </c>
-    </row>
-    <row r="26" ht="15.75" spans="1:6">
+        <v>77.6447111433158</v>
+      </c>
+    </row>
+    <row r="26" ht="15.75" spans="1:5">
       <c r="A26" s="6">
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="5">
+        <v>99.0190028180842</v>
+      </c>
+      <c r="D26" s="5">
+        <v>98.3265985395525</v>
+      </c>
+      <c r="E26" s="5">
+        <v>78.5910079155667</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" spans="1:5">
+      <c r="A27" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="5">
-        <v>100</v>
-      </c>
-      <c r="D26" s="5">
-        <v>100</v>
-      </c>
-      <c r="E26" s="5">
-        <v>82.35</v>
-      </c>
-      <c r="F26" s="5">
-        <v>32.35</v>
-      </c>
-    </row>
-    <row r="27" ht="15.75" spans="1:6">
-      <c r="A27" s="7" t="s">
+      <c r="B27" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="C27" s="7">
-        <v>94.01</v>
+        <v>99.98</v>
       </c>
       <c r="D27" s="7">
-        <v>92.18</v>
+        <v>98.81</v>
       </c>
       <c r="E27" s="7">
-        <v>82.4</v>
-      </c>
-      <c r="F27" s="7">
-        <v>27.4</v>
+        <v>80.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>